<commit_message>
adding in population data
</commit_message>
<xml_diff>
--- a/Filtration project_Whale population and feeding information.xlsx
+++ b/Filtration project_Whale population and feeding information.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/ShirelCh2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA5D2325-CEF1-4F43-963D-0A0D626C9D71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="3060" windowWidth="23640" windowHeight="14340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="3060" windowWidth="23640" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="IUCN 2019 Redlist" sheetId="5" r:id="rId1"/>
@@ -20,23 +14,23 @@
     <sheet name="M. novaeangliae" sheetId="4" r:id="rId5"/>
     <sheet name="Resources" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>IUCN population segments</t>
   </si>
@@ -285,13 +279,37 @@
   </si>
   <si>
     <t>Total removed</t>
+  </si>
+  <si>
+    <t>SpeciesCode</t>
+  </si>
+  <si>
+    <t>bw</t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>bs</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>bb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -763,161 +781,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2">
         <v>10000</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>15537</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>363648</v>
       </c>
-      <c r="F2">
-        <f>D2+E2</f>
+      <c r="G2">
+        <f>E2+F2</f>
         <v>379185</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
         <v>100000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>147607</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>726461</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" si="0">D3+E3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="0">E3+F3</f>
         <v>874068</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4">
         <v>84000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>33585</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>215848</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>249433</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5">
         <v>50000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>86951</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>204589</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>291540</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6">
         <v>80000</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>14049</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>7913</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>21962</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7">
         <v>200000</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>166692</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>166692</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8">
         <v>515000</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>117213</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>117213</v>
       </c>
@@ -933,14 +976,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -1211,26 +1254,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7E5ECD-5C8A-304C-934B-71BBF1709546}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
@@ -1346,14 +1394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
@@ -1489,14 +1537,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
changes made with Shirel
</commit_message>
<xml_diff>
--- a/Filtration project_Whale population and feeding information.xlsx
+++ b/Filtration project_Whale population and feeding information.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsavoca/Documents/Research Data/Whale research/ShirelCh2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FB92D5-0931-704C-B949-B0802EB5F75D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="3060" windowWidth="23640" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="880" yWindow="560" windowWidth="27040" windowHeight="14340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IUCN 2019 Redlist" sheetId="5" r:id="rId1"/>
@@ -14,23 +20,23 @@
     <sheet name="M. novaeangliae" sheetId="4" r:id="rId5"/>
     <sheet name="Resources" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t>IUCN population segments</t>
   </si>
@@ -245,9 +251,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Population estimate</t>
-  </si>
-  <si>
     <t>Balaenoptera musculus</t>
   </si>
   <si>
@@ -269,9 +272,6 @@
     <t>Balaenoptera bonaerensis</t>
   </si>
   <si>
-    <t>Current Range</t>
-  </si>
-  <si>
     <t>Number removed by 20th century whaling (N. Hemisphere)</t>
   </si>
   <si>
@@ -281,35 +281,59 @@
     <t>Total removed</t>
   </si>
   <si>
-    <t>SpeciesCode</t>
-  </si>
-  <si>
-    <t>bw</t>
-  </si>
-  <si>
-    <t>bp</t>
-  </si>
-  <si>
-    <t>mn</t>
-  </si>
-  <si>
-    <t>bs</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>bb</t>
+    <t>CCE population estimate</t>
+  </si>
+  <si>
+    <t>Historical estimate</t>
+  </si>
+  <si>
+    <t>Historical low estimate</t>
+  </si>
+  <si>
+    <t>Historical high estimate</t>
+  </si>
+  <si>
+    <t>Eubalaena glacialis</t>
+  </si>
+  <si>
+    <t>Eubalaena japonica</t>
+  </si>
+  <si>
+    <t>Eubalaena australis</t>
+  </si>
+  <si>
+    <t>Balaena mysticetus</t>
+  </si>
+  <si>
+    <t>Population estimate (Christensen 2006)</t>
+  </si>
+  <si>
+    <t>Population low estimate (Christensen 2006)</t>
+  </si>
+  <si>
+    <t>Population high estimate (Christensen 2006)</t>
+  </si>
+  <si>
+    <t>Population estimate (IUCN 2019)</t>
+  </si>
+  <si>
+    <t>Southern hemisphere population estimate (Christensen 2006)</t>
+  </si>
+  <si>
+    <t>Rocha et al. 2014</t>
+  </si>
+  <si>
+    <t>Whaling numbers</t>
+  </si>
+  <si>
+    <t>Southern hemisphere historic estimate (Christensen 2006)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,10 +384,12 @@
       <name val="Ff1"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF545454"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -781,192 +807,493 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="36.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2">
+        <v>1647</v>
+      </c>
+      <c r="D2">
+        <v>1180</v>
+      </c>
+      <c r="E2">
+        <v>4727</v>
+      </c>
+      <c r="F2">
+        <v>3378</v>
+      </c>
+      <c r="G2">
+        <v>6181</v>
+      </c>
+      <c r="H2">
+        <v>340280</v>
+      </c>
+      <c r="I2">
+        <v>308510</v>
+      </c>
+      <c r="J2">
+        <v>376120</v>
+      </c>
+      <c r="K2">
+        <v>327000</v>
+      </c>
+      <c r="L2">
+        <v>15537</v>
+      </c>
+      <c r="M2">
+        <v>363648</v>
+      </c>
+      <c r="N2">
+        <f>L2+M2</f>
+        <v>379185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2">
-        <v>10000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2">
-        <v>15537</v>
-      </c>
-      <c r="F2">
-        <v>363648</v>
-      </c>
-      <c r="G2">
-        <f>E2+F2</f>
-        <v>379185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>85</v>
+      <c r="B3">
+        <v>100000</v>
       </c>
       <c r="C3">
-        <v>100000</v>
+        <v>9029</v>
+      </c>
+      <c r="D3">
+        <v>55700</v>
       </c>
       <c r="E3">
+        <v>109600</v>
+      </c>
+      <c r="F3">
+        <v>72200</v>
+      </c>
+      <c r="G3">
+        <v>161200</v>
+      </c>
+      <c r="H3">
+        <v>762400</v>
+      </c>
+      <c r="I3">
+        <v>573500</v>
+      </c>
+      <c r="J3">
+        <v>936000</v>
+      </c>
+      <c r="K3">
+        <v>625000</v>
+      </c>
+      <c r="L3">
         <v>147607</v>
       </c>
-      <c r="F3">
+      <c r="M3">
         <v>726461</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">E3+F3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N9" si="0">L3+M3</f>
         <v>874068</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>86</v>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>84000</v>
       </c>
       <c r="C4">
-        <v>84000</v>
+        <v>1918</v>
+      </c>
+      <c r="D4">
+        <v>22500</v>
       </c>
       <c r="E4">
+        <v>42070</v>
+      </c>
+      <c r="F4">
+        <v>31510</v>
+      </c>
+      <c r="G4">
+        <v>59000</v>
+      </c>
+      <c r="H4">
+        <v>231700</v>
+      </c>
+      <c r="I4">
+        <v>154500</v>
+      </c>
+      <c r="J4">
+        <v>285400</v>
+      </c>
+      <c r="K4">
+        <v>199000</v>
+      </c>
+      <c r="L4">
         <v>33585</v>
       </c>
-      <c r="F4">
+      <c r="M4">
         <v>215848</v>
       </c>
-      <c r="G4">
+      <c r="N4">
         <f t="shared" si="0"/>
         <v>249433</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>87</v>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>50000</v>
       </c>
       <c r="C5">
-        <v>50000</v>
+        <v>519</v>
+      </c>
+      <c r="D5">
+        <v>6990</v>
       </c>
       <c r="E5">
+        <v>49090</v>
+      </c>
+      <c r="F5">
+        <v>27780</v>
+      </c>
+      <c r="G5">
+        <v>75740</v>
+      </c>
+      <c r="H5">
+        <v>246000</v>
+      </c>
+      <c r="I5">
+        <v>219020</v>
+      </c>
+      <c r="J5">
+        <v>294400</v>
+      </c>
+      <c r="K5">
+        <v>167000</v>
+      </c>
+      <c r="L5">
         <v>86951</v>
       </c>
-      <c r="F5">
+      <c r="M5">
         <v>204589</v>
       </c>
-      <c r="G5">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>291540</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6">
         <v>80000</v>
       </c>
+      <c r="D6">
+        <v>91300</v>
+      </c>
       <c r="E6">
+        <v>132400</v>
+      </c>
+      <c r="F6">
+        <v>97600</v>
+      </c>
+      <c r="G6">
+        <v>176500</v>
+      </c>
+      <c r="H6">
+        <v>146300</v>
+      </c>
+      <c r="I6">
+        <v>111600</v>
+      </c>
+      <c r="J6">
+        <v>190800</v>
+      </c>
+      <c r="K6">
+        <v>94100</v>
+      </c>
+      <c r="L6">
         <v>14049</v>
       </c>
-      <c r="F6">
+      <c r="M6">
         <v>7913</v>
       </c>
-      <c r="G6">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>21962</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>89</v>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>200000</v>
       </c>
       <c r="C7">
-        <v>200000</v>
+        <v>636</v>
       </c>
       <c r="E7">
+        <v>188900</v>
+      </c>
+      <c r="F7">
+        <v>141900</v>
+      </c>
+      <c r="G7">
+        <v>251400</v>
+      </c>
+      <c r="H7">
+        <v>258000</v>
+      </c>
+      <c r="I7">
+        <v>195700</v>
+      </c>
+      <c r="J7">
+        <v>344300</v>
+      </c>
+      <c r="L7">
         <v>166692</v>
       </c>
-      <c r="G7">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>166692</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8">
         <v>515000</v>
       </c>
+      <c r="D8">
+        <v>318000</v>
+      </c>
+      <c r="E8">
+        <v>318000</v>
+      </c>
       <c r="F8">
+        <v>250000</v>
+      </c>
+      <c r="G8">
+        <v>404000</v>
+      </c>
+      <c r="H8">
+        <v>379000</v>
+      </c>
+      <c r="I8">
+        <v>300000</v>
+      </c>
+      <c r="J8">
+        <v>478000</v>
+      </c>
+      <c r="K8">
+        <v>379000</v>
+      </c>
+      <c r="M8">
         <v>117213</v>
       </c>
-      <c r="G8">
+      <c r="N8">
         <f t="shared" si="0"/>
         <v>117213</v>
       </c>
     </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <v>6740</v>
+      </c>
+      <c r="F9">
+        <v>4580</v>
+      </c>
+      <c r="G9">
+        <v>11100</v>
+      </c>
+      <c r="H9">
+        <v>14100</v>
+      </c>
+      <c r="I9">
+        <v>10100</v>
+      </c>
+      <c r="J9">
+        <v>27800</v>
+      </c>
+      <c r="M9">
+        <v>141</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10">
+        <v>368</v>
+      </c>
+      <c r="F10">
+        <v>257</v>
+      </c>
+      <c r="G10">
+        <v>469</v>
+      </c>
+      <c r="H10">
+        <v>14100</v>
+      </c>
+      <c r="I10">
+        <v>10100</v>
+      </c>
+      <c r="J10">
+        <v>27800</v>
+      </c>
+      <c r="L10">
+        <v>967</v>
+      </c>
+      <c r="N10">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11">
+        <v>6740</v>
+      </c>
+      <c r="E11">
+        <v>368</v>
+      </c>
+      <c r="F11">
+        <v>257</v>
+      </c>
+      <c r="G11">
+        <v>469</v>
+      </c>
+      <c r="H11">
+        <v>86100</v>
+      </c>
+      <c r="I11">
+        <v>73400</v>
+      </c>
+      <c r="J11">
+        <v>98300</v>
+      </c>
+      <c r="K11">
+        <v>86100</v>
+      </c>
+      <c r="M11">
+        <v>4452</v>
+      </c>
+      <c r="N11">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>9450</v>
+      </c>
+      <c r="F12">
+        <v>7500</v>
+      </c>
+      <c r="G12">
+        <v>10800</v>
+      </c>
+      <c r="H12">
+        <v>89000</v>
+      </c>
+      <c r="I12">
+        <v>67000</v>
+      </c>
+      <c r="J12">
+        <v>114000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -976,14 +1303,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="40.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -1254,31 +1581,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7E5ECD-5C8A-304C-934B-71BBF1709546}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
@@ -1394,14 +1716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
@@ -1537,21 +1859,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1559,19 +1881,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>